<commit_message>
changed the stream in the code
</commit_message>
<xml_diff>
--- a/tasks/AnalyticalCase/output/ProjectProductivity.xlsx
+++ b/tasks/AnalyticalCase/output/ProjectProductivity.xlsx
@@ -368,9 +368,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="7.4140625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="19.83984375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="7.46484375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.58984375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="20.19921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -422,10 +422,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>21.86</v>
+        <v>21.860000000000003</v>
       </c>
       <c r="C5" t="n" s="0">
-        <v>5.465</v>
+        <v>5.465000000000001</v>
       </c>
     </row>
     <row r="6">
@@ -466,10 +466,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="n" s="0">
-        <v>31.72</v>
+        <v>31.720000000000006</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>7.93</v>
+        <v>7.9300000000000015</v>
       </c>
     </row>
     <row r="10">
@@ -587,10 +587,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="n" s="0">
-        <v>25.86</v>
+        <v>25.859999999999996</v>
       </c>
       <c r="C20" t="n" s="0">
-        <v>5.172</v>
+        <v>5.171999999999999</v>
       </c>
     </row>
     <row r="21">
@@ -675,10 +675,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="n" s="0">
-        <v>7.96</v>
+        <v>7.959999999999999</v>
       </c>
       <c r="C28" t="n" s="0">
-        <v>2.6533333333333333</v>
+        <v>2.653333333333333</v>
       </c>
     </row>
     <row r="29">
@@ -730,10 +730,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="n" s="0">
-        <v>22.06</v>
+        <v>22.060000000000002</v>
       </c>
       <c r="C33" t="n" s="0">
-        <v>7.353333333333333</v>
+        <v>7.353333333333334</v>
       </c>
     </row>
     <row r="34">
@@ -829,10 +829,10 @@
         <v>43</v>
       </c>
       <c r="B42" t="n" s="0">
-        <v>14.649999999999999</v>
+        <v>14.65</v>
       </c>
       <c r="C42" t="n" s="0">
-        <v>4.883333333333333</v>
+        <v>4.883333333333334</v>
       </c>
     </row>
     <row r="43">
@@ -840,10 +840,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="n" s="0">
-        <v>36.53</v>
+        <v>36.53000000000001</v>
       </c>
       <c r="C43" t="n" s="0">
-        <v>6.088333333333334</v>
+        <v>6.088333333333335</v>
       </c>
     </row>
     <row r="44">
@@ -851,10 +851,10 @@
         <v>45</v>
       </c>
       <c r="B44" t="n" s="0">
-        <v>15.350000000000003</v>
+        <v>15.350000000000001</v>
       </c>
       <c r="C44" t="n" s="0">
-        <v>7.675000000000002</v>
+        <v>7.675000000000001</v>
       </c>
     </row>
     <row r="45">
@@ -862,10 +862,10 @@
         <v>46</v>
       </c>
       <c r="B45" t="n" s="0">
-        <v>16.189999999999998</v>
+        <v>16.19</v>
       </c>
       <c r="C45" t="n" s="0">
-        <v>5.396666666666666</v>
+        <v>5.396666666666667</v>
       </c>
     </row>
     <row r="46">
@@ -972,7 +972,7 @@
         <v>56</v>
       </c>
       <c r="B55" t="n" s="0">
-        <v>13.719999999999999</v>
+        <v>13.72</v>
       </c>
       <c r="C55" t="n" s="0">
         <v>4.573333333333333</v>
@@ -1005,10 +1005,10 @@
         <v>59</v>
       </c>
       <c r="B58" t="n" s="0">
-        <v>11.339999999999998</v>
+        <v>11.34</v>
       </c>
       <c r="C58" t="n" s="0">
-        <v>5.669999999999999</v>
+        <v>5.67</v>
       </c>
     </row>
     <row r="59">
@@ -1071,10 +1071,10 @@
         <v>65</v>
       </c>
       <c r="B64" t="n" s="0">
-        <v>25.84</v>
+        <v>25.840000000000003</v>
       </c>
       <c r="C64" t="n" s="0">
-        <v>5.168</v>
+        <v>5.168000000000001</v>
       </c>
     </row>
     <row r="65">
@@ -1082,10 +1082,10 @@
         <v>66</v>
       </c>
       <c r="B65" t="n" s="0">
-        <v>15.090000000000002</v>
+        <v>15.09</v>
       </c>
       <c r="C65" t="n" s="0">
-        <v>3.7725000000000004</v>
+        <v>3.7725</v>
       </c>
     </row>
     <row r="66">
@@ -1104,7 +1104,7 @@
         <v>68</v>
       </c>
       <c r="B67" t="n" s="0">
-        <v>11.05</v>
+        <v>11.049999999999999</v>
       </c>
       <c r="C67" t="n" s="0">
         <v>2.21</v>
@@ -1148,10 +1148,10 @@
         <v>72</v>
       </c>
       <c r="B71" t="n" s="0">
-        <v>46.12</v>
+        <v>46.120000000000005</v>
       </c>
       <c r="C71" t="n" s="0">
-        <v>6.588571428571428</v>
+        <v>6.588571428571429</v>
       </c>
     </row>
     <row r="72">
@@ -1159,10 +1159,10 @@
         <v>73</v>
       </c>
       <c r="B72" t="n" s="0">
-        <v>47.879999999999995</v>
+        <v>47.88</v>
       </c>
       <c r="C72" t="n" s="0">
-        <v>6.839999999999999</v>
+        <v>6.840000000000001</v>
       </c>
     </row>
     <row r="73">
@@ -1313,7 +1313,7 @@
         <v>87</v>
       </c>
       <c r="B86" t="n" s="0">
-        <v>31.84</v>
+        <v>31.840000000000003</v>
       </c>
       <c r="C86" t="n" s="0">
         <v>6.368</v>
@@ -1357,10 +1357,10 @@
         <v>91</v>
       </c>
       <c r="B90" t="n" s="0">
-        <v>6.119999999999999</v>
+        <v>6.12</v>
       </c>
       <c r="C90" t="n" s="0">
-        <v>2.0399999999999996</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="91">
@@ -1379,7 +1379,7 @@
         <v>93</v>
       </c>
       <c r="B92" t="n" s="0">
-        <v>15.42</v>
+        <v>15.419999999999998</v>
       </c>
       <c r="C92" t="n" s="0">
         <v>5.14</v>
@@ -1390,10 +1390,10 @@
         <v>94</v>
       </c>
       <c r="B93" t="n" s="0">
-        <v>28.27</v>
+        <v>28.270000000000003</v>
       </c>
       <c r="C93" t="n" s="0">
-        <v>5.654</v>
+        <v>5.654000000000001</v>
       </c>
     </row>
     <row r="94">

</xml_diff>